<commit_message>
PPE-105234 : Added test cases. (TCs: PPE-117284, PPE-117285, PPE-117286, PPE-117287, PPE-117288, PPE-117289, PPE-117341, PPE-117432)
</commit_message>
<xml_diff>
--- a/test/pb2/fe/jira/release29/ppe-105234/dev03_bulkimport_invalid.xlsx
+++ b/test/pb2/fe/jira/release29/ppe-105234/dev03_bulkimport_invalid.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>http://www.dev03.webmd.com/men/stick-with-fitness-plan</t>
   </si>
@@ -42,9 +42,6 @@
     <t>http://www.dev03.webmd.com/cancer/tc/pediatric-supportive-care-pdq-supportive-care---patient-information-nci-families</t>
   </si>
   <si>
-    <t>http://www.dev03.webmd.com/cancer/tc/cervical-cancer-screening-topic-overview</t>
-  </si>
-  <si>
     <t>http://www.dev03.webmd.com/fitness-exercise/features/tired-of-exercise</t>
   </si>
   <si>
@@ -82,13 +79,22 @@
   </si>
   <si>
     <t>efgh</t>
+  </si>
+  <si>
+    <t>duplicate</t>
+  </si>
+  <si>
+    <t>loop</t>
+  </si>
+  <si>
+    <t>multihop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -220,6 +226,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -522,7 +536,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -565,13 +579,15 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -605,6 +621,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -912,131 +929,145 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="166.140625" customWidth="1"/>
+    <col min="1" max="1" width="118" customWidth="1"/>
     <col min="2" max="2" width="115" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>15</v>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1"/>
+    <hyperlink ref="B10" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>